<commit_message>
Added jump survey table - unpacking thesis
Signed-off-by: Stefano D'Alessio <stefano496@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/Unpacking/data/Entropy Threshold Survey.xlsx
+++ b/Documentation/Unpacking/data/Entropy Threshold Survey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -104,10 +104,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -298,11 +301,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="80759424"/>
-        <c:axId val="80791424"/>
+        <c:axId val="150894464"/>
+        <c:axId val="150896000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80759424"/>
+        <c:axId val="150894464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -311,7 +314,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80791424"/>
+        <c:crossAx val="150896000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -319,7 +322,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80791424"/>
+        <c:axId val="150896000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -329,7 +332,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80759424"/>
+        <c:crossAx val="150894464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -535,11 +538,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="81859712"/>
-        <c:axId val="81861248"/>
+        <c:axId val="151056384"/>
+        <c:axId val="151057920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81859712"/>
+        <c:axId val="151056384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,7 +551,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81861248"/>
+        <c:crossAx val="151057920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -556,7 +559,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81861248"/>
+        <c:axId val="151057920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -566,7 +569,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81859712"/>
+        <c:crossAx val="151056384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -958,25 +961,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="33.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1123,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>

</xml_diff>